<commit_message>
aligning with code 1
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.location.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.location.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-21T16:23:00-05:00</t>
+    <t>2023-08-03T12:49:33-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -86,7 +86,10 @@
   <si>
     <t>A profile on the Location resource for MHV PHR exposing Location using FHIR API.
 - based on US-Core for Location
-Mapping to [VDIF HospitalLocationTO](StructureDefinition-VA.MHV.PHR.location-mappings.html#mappings-for-vdif-to-mhv-phr-hospitallocationto).</t>
+- `identifier`
+  - system = urn:oid:2.16.840.1.113883.4.349
+- `name` is the name as known
+NOT USING Mapping to [VDIF HospitalLocationTO](StructureDefinition-VA.MHV.PHR.location-mappings.html#mappings-for-vdif-to-mhv-phr-hospitallocationto).</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -3748,7 +3751,7 @@
         <v>38</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>47</v>
@@ -3857,7 +3860,7 @@
         <v>38</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>37</v>
@@ -4077,7 +4080,7 @@
         <v>38</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>37</v>
@@ -4190,7 +4193,7 @@
         <v>38</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>37</v>
@@ -4301,7 +4304,7 @@
         <v>38</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>37</v>
@@ -4414,7 +4417,7 @@
         <v>38</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>37</v>
@@ -4523,7 +4526,7 @@
         <v>38</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>47</v>
@@ -4632,7 +4635,7 @@
         <v>38</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>47</v>
@@ -6071,7 +6074,7 @@
         <v>38</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>37</v>
@@ -6182,7 +6185,7 @@
         <v>38</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>37</v>
@@ -6953,7 +6956,7 @@
         <v>38</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>47</v>
@@ -7066,7 +7069,7 @@
         <v>38</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>37</v>
@@ -7177,7 +7180,7 @@
         <v>38</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>37</v>
@@ -8057,7 +8060,7 @@
         <v>38</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>37</v>
@@ -8166,7 +8169,7 @@
         <v>38</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>37</v>

</xml_diff>